<commit_message>
Changes in RECC_G7IC_V2_0 to include industry. Changes in data input and Config file to correct small errors.
</commit_message>
<xml_diff>
--- a/Data/2_S_RECC_FinalProducts_2015_industry_V1.0.xlsx
+++ b/Data/2_S_RECC_FinalProducts_2015_industry_V1.0.xlsx
@@ -409,9 +409,6 @@
     <t>good g</t>
   </si>
   <si>
-    <t>time t</t>
-  </si>
-  <si>
     <t>Unit of historic stock</t>
   </si>
   <si>
@@ -419,6 +416,9 @@
   </si>
   <si>
     <t>Age-cohort of product c</t>
+  </si>
+  <si>
+    <t>Year t</t>
   </si>
 </sst>
 </file>
@@ -525,7 +525,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -556,6 +556,7 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -863,8 +864,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1187,8 +1188,8 @@
       <c r="C23" s="19" t="s">
         <v>51</v>
       </c>
-      <c r="D23" s="15" t="s">
-        <v>129</v>
+      <c r="D23" s="17" t="s">
+        <v>131</v>
       </c>
       <c r="E23" s="8" t="s">
         <v>53</v>
@@ -1215,7 +1216,7 @@
       <c r="D24" s="7"/>
       <c r="E24" s="8"/>
       <c r="F24" s="17" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="G24" s="10" t="s">
         <v>1</v>
@@ -1267,7 +1268,7 @@
       <c r="A27" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="B27" s="17" t="s">
+      <c r="B27" s="20" t="s">
         <v>132</v>
       </c>
       <c r="G27" s="10" t="s">
@@ -1283,7 +1284,7 @@
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.3">
       <c r="H30" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
   </sheetData>

</xml_diff>